<commit_message>
ship: bulk import improved
</commit_message>
<xml_diff>
--- a/import/bulkTemplate.xlsx
+++ b/import/bulkTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dirk/github/Dans-labs/dariah-contrib/import/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F85CB2-2CAA-494B-A3BE-699A7C3799CE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A69EF5-0E19-8447-9EC2-DC0BFA005405}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28600" windowHeight="20540" activeTab="1" xr2:uid="{9E4E58A0-E663-B14C-8CE3-230EC566B6AD}"/>
+    <workbookView xWindow="0" yWindow="14620" windowWidth="51200" windowHeight="14180" xr2:uid="{9E4E58A0-E663-B14C-8CE3-230EC566B6AD}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="9" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="543">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="544">
   <si>
     <t>title</t>
   </si>
@@ -1549,6 +1549,120 @@
   </si>
   <si>
     <t>*.xslx</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>A legal file name, but no restrictions otherwise</t>
+  </si>
+  <si>
+    <t>AT</t>
+  </si>
+  <si>
+    <t>Austria</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>Croatia</t>
+  </si>
+  <si>
+    <t>CY</t>
+  </si>
+  <si>
+    <t>Cyprus</t>
+  </si>
+  <si>
+    <t>DK</t>
+  </si>
+  <si>
+    <t>Denmark</t>
+  </si>
+  <si>
+    <t>FR</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>GR</t>
+  </si>
+  <si>
+    <t>Greece</t>
+  </si>
+  <si>
+    <t>IE</t>
+  </si>
+  <si>
+    <t>Ireland</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>LU</t>
+  </si>
+  <si>
+    <t>Luxembourg</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>Malta</t>
+  </si>
+  <si>
+    <t>NL</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>PT</t>
+  </si>
+  <si>
+    <t>Portugal</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>Serbia</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>Slovenia</t>
+  </si>
+  <si>
+    <t>PL</t>
+  </si>
+  <si>
+    <t>Poland</t>
+  </si>
+  <si>
+    <t>CZ</t>
+  </si>
+  <si>
+    <t>Czech Republic</t>
+  </si>
+  <si>
+    <t>editors</t>
   </si>
   <si>
     <r>
@@ -1574,7 +1688,49 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">. Each column contains a field of the metadata of the contribution. Most fields are optional, but the </t>
+      <t xml:space="preserve">. Each column contains a field of the metadata of the contribution. Most fields are optional, but the fields </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>country</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>creator, year,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
     </r>
     <r>
       <rPr>
@@ -1596,6 +1752,94 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> must be filled in.
+The field </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>country</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> must be filled in with the 2-letter ISO code for the country that is making the contribution.
+The field </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>year</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is the 4 digit year when the contribution was made to DARIAH.
+The field </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>creator</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is the email address of the creator of the contribution. If the creator has a login for DARIAH, please use the email address belonging to that login. Else, use the email address with which you intend to create a DARIAH account later. Whenever a user with that email address will login into the contribution tool, this contribution will be added to the account of the creator. 
+The optional field </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>editors</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> may be filled with multiple email addresses of users that may edit this record later.
 A number of fields take values from a predefined list. You can enter them by means of a dropdown list. The values of those lists are stored in separate sheets which you can inspect.
 You must choose a value from these lists, except in the case of discipline and keyword, where you may enter new values. 
 In  fields for vcc, email addresses and urls you may enter multiple values, separated by comma and/or newlines (Ctrl+Alt+Enter).
@@ -1625,124 +1869,10 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> must be filled with a number, without a decimal point and without thousand-separators, and without a currency indicator. The amount is taken in € (euros).
-The field country must be filled in with the 2-letter ISO code for the country that is making the contribution.
-The field year is the 4 digit year when the contribution was made to DARIAH.
-The field creator is the email address of the creator of the contribution. If the creator has a login for DARIAH, please use the email address belonging to that login. Else, use the email address with which you intend to create a DARIAH account later. Whenever a user with that email address will login into the contribution tool, this contribution will be added to the account of the creator. 
 Copy this template to a file with a name that contains the country, the year and your EPPN as specified below. That information will be extracted and used for the contributions when they are imported into the system.
 Your EPPN is visible on the interface when you are logged in: click the triangle in front of your name in the top right corner.
 </t>
     </r>
-  </si>
-  <si>
-    <t>*</t>
-  </si>
-  <si>
-    <t>A legal file name, but no restrictions otherwise</t>
-  </si>
-  <si>
-    <t>AT</t>
-  </si>
-  <si>
-    <t>Austria</t>
-  </si>
-  <si>
-    <t>BE</t>
-  </si>
-  <si>
-    <t>HR</t>
-  </si>
-  <si>
-    <t>Croatia</t>
-  </si>
-  <si>
-    <t>CY</t>
-  </si>
-  <si>
-    <t>Cyprus</t>
-  </si>
-  <si>
-    <t>DK</t>
-  </si>
-  <si>
-    <t>Denmark</t>
-  </si>
-  <si>
-    <t>FR</t>
-  </si>
-  <si>
-    <t>France</t>
-  </si>
-  <si>
-    <t>DE</t>
-  </si>
-  <si>
-    <t>Germany</t>
-  </si>
-  <si>
-    <t>GR</t>
-  </si>
-  <si>
-    <t>Greece</t>
-  </si>
-  <si>
-    <t>IE</t>
-  </si>
-  <si>
-    <t>Ireland</t>
-  </si>
-  <si>
-    <t>IT</t>
-  </si>
-  <si>
-    <t>Italy</t>
-  </si>
-  <si>
-    <t>LU</t>
-  </si>
-  <si>
-    <t>Luxembourg</t>
-  </si>
-  <si>
-    <t>MT</t>
-  </si>
-  <si>
-    <t>Malta</t>
-  </si>
-  <si>
-    <t>NL</t>
-  </si>
-  <si>
-    <t>Netherlands</t>
-  </si>
-  <si>
-    <t>PT</t>
-  </si>
-  <si>
-    <t>Portugal</t>
-  </si>
-  <si>
-    <t>RS</t>
-  </si>
-  <si>
-    <t>Serbia</t>
-  </si>
-  <si>
-    <t>SI</t>
-  </si>
-  <si>
-    <t>Slovenia</t>
-  </si>
-  <si>
-    <t>PL</t>
-  </si>
-  <si>
-    <t>Poland</t>
-  </si>
-  <si>
-    <t>CZ</t>
-  </si>
-  <si>
-    <t>Czech Republic</t>
   </si>
 </sst>
 </file>
@@ -2140,8 +2270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06979413-2D2E-A04C-B6B8-B332E67D4E2B}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2149,7 +2279,7 @@
     <col min="1" max="1" width="10.83203125" style="7"/>
     <col min="2" max="2" width="52" style="7" customWidth="1"/>
     <col min="3" max="3" width="22.33203125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="50" style="7" customWidth="1"/>
+    <col min="4" max="4" width="81.1640625" style="7" customWidth="1"/>
     <col min="5" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
@@ -2158,7 +2288,7 @@
         <v>498</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>505</v>
+        <v>543</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -2173,10 +2303,10 @@
     </row>
     <row r="3" spans="1:4" ht="17">
       <c r="C3" s="7" t="s">
+        <v>505</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>506</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>507</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17">
@@ -3997,7 +4127,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{011AAF7A-1E9C-5B46-9840-3958C3A5B983}">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -4005,15 +4135,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>507</v>
+      </c>
+      <c r="B1" t="s">
         <v>508</v>
-      </c>
-      <c r="B1" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B2" t="s">
         <v>181</v>
@@ -4021,130 +4151,130 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
+        <v>510</v>
+      </c>
+      <c r="B3" t="s">
         <v>511</v>
-      </c>
-      <c r="B3" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
+        <v>512</v>
+      </c>
+      <c r="B4" t="s">
         <v>513</v>
-      </c>
-      <c r="B4" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
+        <v>540</v>
+      </c>
+      <c r="B5" t="s">
         <v>541</v>
-      </c>
-      <c r="B5" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
+        <v>514</v>
+      </c>
+      <c r="B6" t="s">
         <v>515</v>
-      </c>
-      <c r="B6" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
+        <v>516</v>
+      </c>
+      <c r="B7" t="s">
         <v>517</v>
-      </c>
-      <c r="B7" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
+        <v>518</v>
+      </c>
+      <c r="B8" t="s">
         <v>519</v>
-      </c>
-      <c r="B8" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
+        <v>520</v>
+      </c>
+      <c r="B9" t="s">
         <v>521</v>
-      </c>
-      <c r="B9" t="s">
-        <v>522</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
+        <v>522</v>
+      </c>
+      <c r="B10" t="s">
         <v>523</v>
-      </c>
-      <c r="B10" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
+        <v>524</v>
+      </c>
+      <c r="B11" t="s">
         <v>525</v>
-      </c>
-      <c r="B11" t="s">
-        <v>526</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
+        <v>526</v>
+      </c>
+      <c r="B12" t="s">
         <v>527</v>
-      </c>
-      <c r="B12" t="s">
-        <v>528</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
+        <v>528</v>
+      </c>
+      <c r="B13" t="s">
         <v>529</v>
-      </c>
-      <c r="B13" t="s">
-        <v>530</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
+        <v>530</v>
+      </c>
+      <c r="B14" t="s">
         <v>531</v>
-      </c>
-      <c r="B14" t="s">
-        <v>532</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
+        <v>532</v>
+      </c>
+      <c r="B15" t="s">
         <v>533</v>
-      </c>
-      <c r="B15" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
+        <v>534</v>
+      </c>
+      <c r="B16" t="s">
         <v>535</v>
-      </c>
-      <c r="B16" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
+        <v>536</v>
+      </c>
+      <c r="B17" t="s">
         <v>537</v>
-      </c>
-      <c r="B17" t="s">
-        <v>538</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
+        <v>538</v>
+      </c>
+      <c r="B18" t="s">
         <v>539</v>
-      </c>
-      <c r="B18" t="s">
-        <v>540</v>
       </c>
     </row>
   </sheetData>
@@ -4154,31 +4284,31 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{795743C0-90E8-1647-AA07-019994BABA6A}">
-  <dimension ref="A1:R129"/>
+  <dimension ref="A1:S129"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E92" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F92" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C140" sqref="C140"/>
+      <selection pane="bottomRight" activeCell="D94" sqref="D94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="3" width="10.83203125" style="4"/>
-    <col min="4" max="4" width="30" style="4" customWidth="1"/>
-    <col min="5" max="6" width="17.83203125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="66.5" style="4" customWidth="1"/>
-    <col min="8" max="8" width="16.83203125" style="4" customWidth="1"/>
-    <col min="9" max="9" width="46.33203125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="17.83203125" style="4" customWidth="1"/>
-    <col min="11" max="11" width="17.5" style="4" customWidth="1"/>
-    <col min="12" max="12" width="30.1640625" style="4" customWidth="1"/>
-    <col min="13" max="13" width="22.33203125" style="4" customWidth="1"/>
-    <col min="14" max="16384" width="10.83203125" style="4"/>
+    <col min="1" max="4" width="10.83203125" style="4"/>
+    <col min="5" max="5" width="30" style="4" customWidth="1"/>
+    <col min="6" max="7" width="17.83203125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="66.5" style="4" customWidth="1"/>
+    <col min="9" max="9" width="16.83203125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="46.33203125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="17.83203125" style="4" customWidth="1"/>
+    <col min="12" max="12" width="17.5" style="4" customWidth="1"/>
+    <col min="13" max="13" width="30.1640625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="22.33203125" style="4" customWidth="1"/>
+    <col min="15" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="3" customFormat="1" ht="35" customHeight="1">
+    <row r="1" spans="1:19" s="3" customFormat="1" ht="35" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>501</v>
       </c>
@@ -4189,818 +4319,821 @@
         <v>503</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>542</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>488</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>499</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>500</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
-      <c r="G2" s="5"/>
+    <row r="2" spans="1:19">
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
-      <c r="J2" s="2"/>
-    </row>
-    <row r="3" spans="1:18">
-      <c r="G3" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="1:19">
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
-      <c r="J3" s="2"/>
-    </row>
-    <row r="4" spans="1:18">
-      <c r="G4" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="1:19">
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:18">
-      <c r="G5" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="1:19">
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
-      <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="1:18">
-      <c r="G6" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:19">
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:18">
-      <c r="G7" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:19">
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
-      <c r="J7" s="2"/>
-    </row>
-    <row r="8" spans="1:18">
-      <c r="G8" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:19">
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
-      <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="1:18">
-      <c r="G9" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:19">
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
-      <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:18">
-      <c r="G10" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:19">
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
-      <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="1:18">
-      <c r="G11" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:19">
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
-      <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="1:18">
-      <c r="G12" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:19">
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
-      <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="1:18">
-      <c r="G13" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:19">
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
-      <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="1:18">
-      <c r="G14" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:19">
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
-      <c r="J14" s="2"/>
-    </row>
-    <row r="15" spans="1:18">
-      <c r="G15" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:19">
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
-      <c r="J15" s="2"/>
-    </row>
-    <row r="16" spans="1:18">
-      <c r="G16" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:19">
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
-      <c r="J16" s="2"/>
-    </row>
-    <row r="17" spans="7:10">
-      <c r="G17" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="8:11">
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
-      <c r="J17" s="2"/>
-    </row>
-    <row r="18" spans="7:10">
-      <c r="G18" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="8:11">
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
-      <c r="J18" s="2"/>
-    </row>
-    <row r="19" spans="7:10">
-      <c r="G19" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="8:11">
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
-      <c r="J19" s="2"/>
-    </row>
-    <row r="20" spans="7:10">
-      <c r="G20" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="8:11">
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
-      <c r="J20" s="2"/>
-    </row>
-    <row r="21" spans="7:10">
-      <c r="G21" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="8:11">
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="2"/>
-    </row>
-    <row r="22" spans="7:10">
-      <c r="G22" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="8:11">
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
-      <c r="J22" s="2"/>
-    </row>
-    <row r="23" spans="7:10">
-      <c r="G23" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="2"/>
+    </row>
+    <row r="23" spans="8:11">
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
-      <c r="J23" s="2"/>
-    </row>
-    <row r="24" spans="7:10">
-      <c r="G24" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="2"/>
+    </row>
+    <row r="24" spans="8:11">
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
-      <c r="J24" s="2"/>
-    </row>
-    <row r="25" spans="7:10">
-      <c r="G25" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="2"/>
+    </row>
+    <row r="25" spans="8:11">
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
-      <c r="J25" s="2"/>
-    </row>
-    <row r="26" spans="7:10">
-      <c r="G26" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="2"/>
+    </row>
+    <row r="26" spans="8:11">
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
-      <c r="J26" s="2"/>
-    </row>
-    <row r="27" spans="7:10">
-      <c r="G27" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="2"/>
+    </row>
+    <row r="27" spans="8:11">
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
-      <c r="J27" s="2"/>
-    </row>
-    <row r="28" spans="7:10">
-      <c r="G28" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="2"/>
+    </row>
+    <row r="28" spans="8:11">
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
-      <c r="J28" s="2"/>
-    </row>
-    <row r="29" spans="7:10">
-      <c r="G29" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="2"/>
+    </row>
+    <row r="29" spans="8:11">
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
-      <c r="J29" s="2"/>
-    </row>
-    <row r="30" spans="7:10">
-      <c r="G30" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="2"/>
+    </row>
+    <row r="30" spans="8:11">
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
-      <c r="J30" s="2"/>
-    </row>
-    <row r="31" spans="7:10">
-      <c r="G31" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="2"/>
+    </row>
+    <row r="31" spans="8:11">
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
-      <c r="J31" s="2"/>
-    </row>
-    <row r="32" spans="7:10">
-      <c r="G32" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="2"/>
+    </row>
+    <row r="32" spans="8:11">
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
-      <c r="J32" s="2"/>
-    </row>
-    <row r="33" spans="7:10">
-      <c r="G33" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="2"/>
+    </row>
+    <row r="33" spans="8:11">
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
-      <c r="J33" s="2"/>
-    </row>
-    <row r="34" spans="7:10">
-      <c r="G34" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="2"/>
+    </row>
+    <row r="34" spans="8:11">
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
-      <c r="J34" s="2"/>
-    </row>
-    <row r="35" spans="7:10">
-      <c r="G35" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="2"/>
+    </row>
+    <row r="35" spans="8:11">
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
-      <c r="J35" s="2"/>
-    </row>
-    <row r="36" spans="7:10">
-      <c r="G36" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="2"/>
+    </row>
+    <row r="36" spans="8:11">
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
-      <c r="J36" s="2"/>
-    </row>
-    <row r="37" spans="7:10">
-      <c r="G37" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="2"/>
+    </row>
+    <row r="37" spans="8:11">
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
-      <c r="J37" s="2"/>
-    </row>
-    <row r="38" spans="7:10">
-      <c r="G38" s="5"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="2"/>
+    </row>
+    <row r="38" spans="8:11">
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
-      <c r="J38" s="2"/>
-    </row>
-    <row r="39" spans="7:10">
-      <c r="G39" s="5"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="2"/>
+    </row>
+    <row r="39" spans="8:11">
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
-      <c r="J39" s="2"/>
-    </row>
-    <row r="40" spans="7:10">
-      <c r="G40" s="5"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="2"/>
+    </row>
+    <row r="40" spans="8:11">
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
-      <c r="J40" s="2"/>
-    </row>
-    <row r="41" spans="7:10">
-      <c r="G41" s="5"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="2"/>
+    </row>
+    <row r="41" spans="8:11">
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>
-      <c r="J41" s="2"/>
-    </row>
-    <row r="42" spans="7:10">
-      <c r="G42" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="2"/>
+    </row>
+    <row r="42" spans="8:11">
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
-      <c r="J42" s="2"/>
-    </row>
-    <row r="43" spans="7:10">
-      <c r="G43" s="5"/>
+      <c r="J42" s="5"/>
+      <c r="K42" s="2"/>
+    </row>
+    <row r="43" spans="8:11">
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
-      <c r="J43" s="2"/>
-    </row>
-    <row r="44" spans="7:10">
-      <c r="G44" s="5"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="2"/>
+    </row>
+    <row r="44" spans="8:11">
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
-      <c r="J44" s="2"/>
-    </row>
-    <row r="45" spans="7:10">
-      <c r="G45" s="5"/>
+      <c r="J44" s="5"/>
+      <c r="K44" s="2"/>
+    </row>
+    <row r="45" spans="8:11">
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
-      <c r="J45" s="2"/>
-    </row>
-    <row r="46" spans="7:10">
-      <c r="G46" s="5"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="2"/>
+    </row>
+    <row r="46" spans="8:11">
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
-      <c r="J46" s="2"/>
-    </row>
-    <row r="47" spans="7:10">
-      <c r="G47" s="5"/>
+      <c r="J46" s="5"/>
+      <c r="K46" s="2"/>
+    </row>
+    <row r="47" spans="8:11">
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
-      <c r="J47" s="2"/>
-    </row>
-    <row r="48" spans="7:10">
-      <c r="G48" s="5"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="2"/>
+    </row>
+    <row r="48" spans="8:11">
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
-      <c r="J48" s="2"/>
-    </row>
-    <row r="49" spans="7:10">
-      <c r="G49" s="5"/>
+      <c r="J48" s="5"/>
+      <c r="K48" s="2"/>
+    </row>
+    <row r="49" spans="8:11">
       <c r="H49" s="5"/>
       <c r="I49" s="5"/>
-      <c r="J49" s="2"/>
-    </row>
-    <row r="50" spans="7:10">
-      <c r="G50" s="5"/>
+      <c r="J49" s="5"/>
+      <c r="K49" s="2"/>
+    </row>
+    <row r="50" spans="8:11">
       <c r="H50" s="5"/>
       <c r="I50" s="5"/>
-      <c r="J50" s="2"/>
-    </row>
-    <row r="51" spans="7:10">
-      <c r="G51" s="5"/>
+      <c r="J50" s="5"/>
+      <c r="K50" s="2"/>
+    </row>
+    <row r="51" spans="8:11">
       <c r="H51" s="5"/>
       <c r="I51" s="5"/>
-      <c r="J51" s="2"/>
-    </row>
-    <row r="52" spans="7:10">
-      <c r="G52" s="5"/>
+      <c r="J51" s="5"/>
+      <c r="K51" s="2"/>
+    </row>
+    <row r="52" spans="8:11">
       <c r="H52" s="5"/>
       <c r="I52" s="5"/>
-      <c r="J52" s="2"/>
-    </row>
-    <row r="53" spans="7:10">
-      <c r="G53" s="5"/>
+      <c r="J52" s="5"/>
+      <c r="K52" s="2"/>
+    </row>
+    <row r="53" spans="8:11">
       <c r="H53" s="5"/>
       <c r="I53" s="5"/>
-      <c r="J53" s="2"/>
-    </row>
-    <row r="54" spans="7:10">
-      <c r="G54" s="5"/>
+      <c r="J53" s="5"/>
+      <c r="K53" s="2"/>
+    </row>
+    <row r="54" spans="8:11">
       <c r="H54" s="5"/>
       <c r="I54" s="5"/>
-      <c r="J54" s="2"/>
-    </row>
-    <row r="55" spans="7:10">
-      <c r="G55" s="5"/>
+      <c r="J54" s="5"/>
+      <c r="K54" s="2"/>
+    </row>
+    <row r="55" spans="8:11">
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
-      <c r="J55" s="2"/>
-    </row>
-    <row r="56" spans="7:10">
-      <c r="G56" s="5"/>
+      <c r="J55" s="5"/>
+      <c r="K55" s="2"/>
+    </row>
+    <row r="56" spans="8:11">
       <c r="H56" s="5"/>
       <c r="I56" s="5"/>
-      <c r="J56" s="2"/>
-    </row>
-    <row r="57" spans="7:10">
-      <c r="G57" s="5"/>
+      <c r="J56" s="5"/>
+      <c r="K56" s="2"/>
+    </row>
+    <row r="57" spans="8:11">
       <c r="H57" s="5"/>
       <c r="I57" s="5"/>
-      <c r="J57" s="2"/>
-    </row>
-    <row r="58" spans="7:10">
-      <c r="G58" s="5"/>
+      <c r="J57" s="5"/>
+      <c r="K57" s="2"/>
+    </row>
+    <row r="58" spans="8:11">
       <c r="H58" s="5"/>
       <c r="I58" s="5"/>
-      <c r="J58" s="2"/>
-    </row>
-    <row r="59" spans="7:10">
-      <c r="G59" s="5"/>
+      <c r="J58" s="5"/>
+      <c r="K58" s="2"/>
+    </row>
+    <row r="59" spans="8:11">
       <c r="H59" s="5"/>
       <c r="I59" s="5"/>
-      <c r="J59" s="2"/>
-    </row>
-    <row r="60" spans="7:10">
-      <c r="G60" s="5"/>
+      <c r="J59" s="5"/>
+      <c r="K59" s="2"/>
+    </row>
+    <row r="60" spans="8:11">
       <c r="H60" s="5"/>
       <c r="I60" s="5"/>
-      <c r="J60" s="2"/>
-    </row>
-    <row r="61" spans="7:10">
-      <c r="G61" s="5"/>
+      <c r="J60" s="5"/>
+      <c r="K60" s="2"/>
+    </row>
+    <row r="61" spans="8:11">
       <c r="H61" s="5"/>
       <c r="I61" s="5"/>
-      <c r="J61" s="2"/>
-    </row>
-    <row r="62" spans="7:10">
-      <c r="G62" s="5"/>
+      <c r="J61" s="5"/>
+      <c r="K61" s="2"/>
+    </row>
+    <row r="62" spans="8:11">
       <c r="H62" s="5"/>
       <c r="I62" s="5"/>
-      <c r="J62" s="2"/>
-    </row>
-    <row r="63" spans="7:10">
-      <c r="G63" s="5"/>
+      <c r="J62" s="5"/>
+      <c r="K62" s="2"/>
+    </row>
+    <row r="63" spans="8:11">
       <c r="H63" s="5"/>
       <c r="I63" s="5"/>
-      <c r="J63" s="2"/>
-    </row>
-    <row r="64" spans="7:10">
-      <c r="G64" s="5"/>
+      <c r="J63" s="5"/>
+      <c r="K63" s="2"/>
+    </row>
+    <row r="64" spans="8:11">
       <c r="H64" s="5"/>
       <c r="I64" s="5"/>
-      <c r="J64" s="2"/>
-    </row>
-    <row r="65" spans="7:10">
-      <c r="G65" s="5"/>
+      <c r="J64" s="5"/>
+      <c r="K64" s="2"/>
+    </row>
+    <row r="65" spans="8:11">
       <c r="H65" s="5"/>
       <c r="I65" s="5"/>
-      <c r="J65" s="2"/>
-    </row>
-    <row r="66" spans="7:10">
-      <c r="G66" s="5"/>
+      <c r="J65" s="5"/>
+      <c r="K65" s="2"/>
+    </row>
+    <row r="66" spans="8:11">
       <c r="H66" s="5"/>
       <c r="I66" s="5"/>
-      <c r="J66" s="2"/>
-    </row>
-    <row r="67" spans="7:10">
-      <c r="G67" s="5"/>
+      <c r="J66" s="5"/>
+      <c r="K66" s="2"/>
+    </row>
+    <row r="67" spans="8:11">
       <c r="H67" s="5"/>
       <c r="I67" s="5"/>
-      <c r="J67" s="2"/>
-    </row>
-    <row r="68" spans="7:10">
-      <c r="G68" s="5"/>
+      <c r="J67" s="5"/>
+      <c r="K67" s="2"/>
+    </row>
+    <row r="68" spans="8:11">
       <c r="H68" s="5"/>
       <c r="I68" s="5"/>
-      <c r="J68" s="2"/>
-    </row>
-    <row r="69" spans="7:10">
-      <c r="G69" s="5"/>
+      <c r="J68" s="5"/>
+      <c r="K68" s="2"/>
+    </row>
+    <row r="69" spans="8:11">
       <c r="H69" s="5"/>
       <c r="I69" s="5"/>
-      <c r="J69" s="2"/>
-    </row>
-    <row r="70" spans="7:10">
-      <c r="G70" s="5"/>
+      <c r="J69" s="5"/>
+      <c r="K69" s="2"/>
+    </row>
+    <row r="70" spans="8:11">
       <c r="H70" s="5"/>
       <c r="I70" s="5"/>
-      <c r="J70" s="2"/>
-    </row>
-    <row r="71" spans="7:10">
-      <c r="G71" s="5"/>
+      <c r="J70" s="5"/>
+      <c r="K70" s="2"/>
+    </row>
+    <row r="71" spans="8:11">
       <c r="H71" s="5"/>
       <c r="I71" s="5"/>
-      <c r="J71" s="2"/>
-    </row>
-    <row r="72" spans="7:10">
-      <c r="G72" s="5"/>
+      <c r="J71" s="5"/>
+      <c r="K71" s="2"/>
+    </row>
+    <row r="72" spans="8:11">
       <c r="H72" s="5"/>
       <c r="I72" s="5"/>
-      <c r="J72" s="2"/>
-    </row>
-    <row r="73" spans="7:10">
-      <c r="G73" s="5"/>
+      <c r="J72" s="5"/>
+      <c r="K72" s="2"/>
+    </row>
+    <row r="73" spans="8:11">
       <c r="H73" s="5"/>
       <c r="I73" s="5"/>
-      <c r="J73" s="2"/>
-    </row>
-    <row r="74" spans="7:10">
-      <c r="G74" s="5"/>
+      <c r="J73" s="5"/>
+      <c r="K73" s="2"/>
+    </row>
+    <row r="74" spans="8:11">
       <c r="H74" s="5"/>
       <c r="I74" s="5"/>
-      <c r="J74" s="2"/>
-    </row>
-    <row r="75" spans="7:10">
-      <c r="G75" s="5"/>
+      <c r="J74" s="5"/>
+      <c r="K74" s="2"/>
+    </row>
+    <row r="75" spans="8:11">
       <c r="H75" s="5"/>
       <c r="I75" s="5"/>
-      <c r="J75" s="2"/>
-    </row>
-    <row r="76" spans="7:10">
-      <c r="G76" s="5"/>
+      <c r="J75" s="5"/>
+      <c r="K75" s="2"/>
+    </row>
+    <row r="76" spans="8:11">
       <c r="H76" s="5"/>
       <c r="I76" s="5"/>
-      <c r="J76" s="2"/>
-    </row>
-    <row r="77" spans="7:10">
-      <c r="G77" s="5"/>
+      <c r="J76" s="5"/>
+      <c r="K76" s="2"/>
+    </row>
+    <row r="77" spans="8:11">
       <c r="H77" s="5"/>
       <c r="I77" s="5"/>
-      <c r="J77" s="2"/>
-    </row>
-    <row r="78" spans="7:10">
-      <c r="G78" s="5"/>
+      <c r="J77" s="5"/>
+      <c r="K77" s="2"/>
+    </row>
+    <row r="78" spans="8:11">
       <c r="H78" s="5"/>
       <c r="I78" s="5"/>
-      <c r="J78" s="2"/>
-    </row>
-    <row r="79" spans="7:10">
-      <c r="G79" s="5"/>
+      <c r="J78" s="5"/>
+      <c r="K78" s="2"/>
+    </row>
+    <row r="79" spans="8:11">
       <c r="H79" s="5"/>
       <c r="I79" s="5"/>
-      <c r="J79" s="2"/>
-    </row>
-    <row r="80" spans="7:10">
-      <c r="G80" s="5"/>
+      <c r="J79" s="5"/>
+      <c r="K79" s="2"/>
+    </row>
+    <row r="80" spans="8:11">
       <c r="H80" s="5"/>
       <c r="I80" s="5"/>
-      <c r="J80" s="2"/>
-    </row>
-    <row r="81" spans="7:10">
-      <c r="G81" s="5"/>
+      <c r="J80" s="5"/>
+      <c r="K80" s="2"/>
+    </row>
+    <row r="81" spans="8:11">
       <c r="H81" s="5"/>
       <c r="I81" s="5"/>
-      <c r="J81" s="2"/>
-    </row>
-    <row r="82" spans="7:10">
-      <c r="G82" s="5"/>
+      <c r="J81" s="5"/>
+      <c r="K81" s="2"/>
+    </row>
+    <row r="82" spans="8:11">
       <c r="H82" s="5"/>
       <c r="I82" s="5"/>
-      <c r="J82" s="2"/>
-    </row>
-    <row r="83" spans="7:10">
-      <c r="G83" s="5"/>
+      <c r="J82" s="5"/>
+      <c r="K82" s="2"/>
+    </row>
+    <row r="83" spans="8:11">
       <c r="H83" s="5"/>
       <c r="I83" s="5"/>
-      <c r="J83" s="2"/>
-    </row>
-    <row r="84" spans="7:10">
-      <c r="G84" s="5"/>
+      <c r="J83" s="5"/>
+      <c r="K83" s="2"/>
+    </row>
+    <row r="84" spans="8:11">
       <c r="H84" s="5"/>
       <c r="I84" s="5"/>
-      <c r="J84" s="2"/>
-    </row>
-    <row r="85" spans="7:10">
-      <c r="G85" s="5"/>
+      <c r="J84" s="5"/>
+      <c r="K84" s="2"/>
+    </row>
+    <row r="85" spans="8:11">
       <c r="H85" s="5"/>
       <c r="I85" s="5"/>
-      <c r="J85" s="2"/>
-    </row>
-    <row r="86" spans="7:10">
-      <c r="G86" s="5"/>
+      <c r="J85" s="5"/>
+      <c r="K85" s="2"/>
+    </row>
+    <row r="86" spans="8:11">
       <c r="H86" s="5"/>
       <c r="I86" s="5"/>
-      <c r="J86" s="2"/>
-    </row>
-    <row r="87" spans="7:10">
-      <c r="G87" s="5"/>
+      <c r="J86" s="5"/>
+      <c r="K86" s="2"/>
+    </row>
+    <row r="87" spans="8:11">
       <c r="H87" s="5"/>
       <c r="I87" s="5"/>
-      <c r="J87" s="2"/>
-    </row>
-    <row r="88" spans="7:10">
-      <c r="G88" s="5"/>
+      <c r="J87" s="5"/>
+      <c r="K87" s="2"/>
+    </row>
+    <row r="88" spans="8:11">
       <c r="H88" s="5"/>
       <c r="I88" s="5"/>
-      <c r="J88" s="2"/>
-    </row>
-    <row r="89" spans="7:10">
-      <c r="G89" s="5"/>
+      <c r="J88" s="5"/>
+      <c r="K88" s="2"/>
+    </row>
+    <row r="89" spans="8:11">
       <c r="H89" s="5"/>
       <c r="I89" s="5"/>
-      <c r="J89" s="2"/>
-    </row>
-    <row r="90" spans="7:10">
-      <c r="G90" s="5"/>
+      <c r="J89" s="5"/>
+      <c r="K89" s="2"/>
+    </row>
+    <row r="90" spans="8:11">
       <c r="H90" s="5"/>
       <c r="I90" s="5"/>
-      <c r="J90" s="2"/>
-    </row>
-    <row r="91" spans="7:10">
-      <c r="G91" s="5"/>
+      <c r="J90" s="5"/>
+      <c r="K90" s="2"/>
+    </row>
+    <row r="91" spans="8:11">
       <c r="H91" s="5"/>
       <c r="I91" s="5"/>
-      <c r="J91" s="2"/>
-    </row>
-    <row r="92" spans="7:10">
-      <c r="G92" s="5"/>
+      <c r="J91" s="5"/>
+      <c r="K91" s="2"/>
+    </row>
+    <row r="92" spans="8:11">
       <c r="H92" s="5"/>
       <c r="I92" s="5"/>
-      <c r="J92" s="2"/>
-    </row>
-    <row r="93" spans="7:10">
-      <c r="G93" s="5"/>
+      <c r="J92" s="5"/>
+      <c r="K92" s="2"/>
+    </row>
+    <row r="93" spans="8:11">
       <c r="H93" s="5"/>
       <c r="I93" s="5"/>
-      <c r="J93" s="2"/>
-    </row>
-    <row r="94" spans="7:10">
-      <c r="G94" s="5"/>
+      <c r="J93" s="5"/>
+      <c r="K93" s="2"/>
+    </row>
+    <row r="94" spans="8:11">
       <c r="H94" s="5"/>
       <c r="I94" s="5"/>
-      <c r="J94" s="2"/>
-    </row>
-    <row r="95" spans="7:10">
-      <c r="G95" s="5"/>
+      <c r="J94" s="5"/>
+      <c r="K94" s="2"/>
+    </row>
+    <row r="95" spans="8:11">
       <c r="H95" s="5"/>
       <c r="I95" s="5"/>
-      <c r="J95" s="2"/>
-    </row>
-    <row r="96" spans="7:10">
-      <c r="G96" s="5"/>
+      <c r="J95" s="5"/>
+      <c r="K95" s="2"/>
+    </row>
+    <row r="96" spans="8:11">
       <c r="H96" s="5"/>
       <c r="I96" s="5"/>
-      <c r="J96" s="2"/>
-    </row>
-    <row r="97" spans="7:10">
-      <c r="G97" s="5"/>
+      <c r="J96" s="5"/>
+      <c r="K96" s="2"/>
+    </row>
+    <row r="97" spans="8:11">
       <c r="H97" s="5"/>
       <c r="I97" s="5"/>
-      <c r="J97" s="2"/>
-    </row>
-    <row r="98" spans="7:10">
-      <c r="G98" s="5"/>
+      <c r="J97" s="5"/>
+      <c r="K97" s="2"/>
+    </row>
+    <row r="98" spans="8:11">
       <c r="H98" s="5"/>
       <c r="I98" s="5"/>
-      <c r="J98" s="2"/>
-    </row>
-    <row r="99" spans="7:10">
-      <c r="G99" s="5"/>
+      <c r="J98" s="5"/>
+      <c r="K98" s="2"/>
+    </row>
+    <row r="99" spans="8:11">
       <c r="H99" s="5"/>
       <c r="I99" s="5"/>
-      <c r="J99" s="2"/>
-    </row>
-    <row r="100" spans="7:10">
-      <c r="G100" s="5"/>
+      <c r="J99" s="5"/>
+      <c r="K99" s="2"/>
+    </row>
+    <row r="100" spans="8:11">
       <c r="H100" s="5"/>
       <c r="I100" s="5"/>
-      <c r="J100" s="2"/>
-    </row>
-    <row r="101" spans="7:10">
-      <c r="G101" s="5"/>
+      <c r="J100" s="5"/>
+      <c r="K100" s="2"/>
+    </row>
+    <row r="101" spans="8:11">
       <c r="H101" s="5"/>
       <c r="I101" s="5"/>
-      <c r="J101" s="2"/>
-    </row>
-    <row r="102" spans="7:10">
-      <c r="G102" s="5"/>
+      <c r="J101" s="5"/>
+      <c r="K101" s="2"/>
+    </row>
+    <row r="102" spans="8:11">
       <c r="H102" s="5"/>
       <c r="I102" s="5"/>
-      <c r="J102" s="2"/>
-    </row>
-    <row r="103" spans="7:10">
-      <c r="G103" s="5"/>
+      <c r="J102" s="5"/>
+      <c r="K102" s="2"/>
+    </row>
+    <row r="103" spans="8:11">
       <c r="H103" s="5"/>
       <c r="I103" s="5"/>
-      <c r="J103" s="2"/>
-    </row>
-    <row r="104" spans="7:10">
-      <c r="G104" s="5"/>
+      <c r="J103" s="5"/>
+      <c r="K103" s="2"/>
+    </row>
+    <row r="104" spans="8:11">
       <c r="H104" s="5"/>
       <c r="I104" s="5"/>
-      <c r="J104" s="2"/>
-    </row>
-    <row r="105" spans="7:10">
-      <c r="G105" s="5"/>
+      <c r="J104" s="5"/>
+      <c r="K104" s="2"/>
+    </row>
+    <row r="105" spans="8:11">
       <c r="H105" s="5"/>
       <c r="I105" s="5"/>
-      <c r="J105" s="2"/>
-    </row>
-    <row r="106" spans="7:10">
-      <c r="G106" s="5"/>
+      <c r="J105" s="5"/>
+      <c r="K105" s="2"/>
+    </row>
+    <row r="106" spans="8:11">
       <c r="H106" s="5"/>
       <c r="I106" s="5"/>
-      <c r="J106" s="2"/>
-    </row>
-    <row r="107" spans="7:10">
-      <c r="G107" s="5"/>
+      <c r="J106" s="5"/>
+      <c r="K106" s="2"/>
+    </row>
+    <row r="107" spans="8:11">
       <c r="H107" s="5"/>
       <c r="I107" s="5"/>
-      <c r="J107" s="2"/>
-    </row>
-    <row r="108" spans="7:10">
-      <c r="G108" s="5"/>
+      <c r="J107" s="5"/>
+      <c r="K107" s="2"/>
+    </row>
+    <row r="108" spans="8:11">
       <c r="H108" s="5"/>
       <c r="I108" s="5"/>
-      <c r="J108" s="2"/>
-    </row>
-    <row r="109" spans="7:10">
-      <c r="G109" s="5"/>
+      <c r="J108" s="5"/>
+      <c r="K108" s="2"/>
+    </row>
+    <row r="109" spans="8:11">
       <c r="H109" s="5"/>
       <c r="I109" s="5"/>
-      <c r="J109" s="2"/>
-    </row>
-    <row r="110" spans="7:10">
-      <c r="G110" s="5"/>
+      <c r="J109" s="5"/>
+      <c r="K109" s="2"/>
+    </row>
+    <row r="110" spans="8:11">
       <c r="H110" s="5"/>
       <c r="I110" s="5"/>
-      <c r="J110" s="2"/>
-    </row>
-    <row r="111" spans="7:10">
-      <c r="G111" s="5"/>
+      <c r="J110" s="5"/>
+      <c r="K110" s="2"/>
+    </row>
+    <row r="111" spans="8:11">
       <c r="H111" s="5"/>
       <c r="I111" s="5"/>
-      <c r="J111" s="2"/>
-    </row>
-    <row r="112" spans="7:10">
-      <c r="G112" s="5"/>
+      <c r="J111" s="5"/>
+      <c r="K111" s="2"/>
+    </row>
+    <row r="112" spans="8:11">
       <c r="H112" s="5"/>
       <c r="I112" s="5"/>
-      <c r="J112" s="2"/>
-    </row>
-    <row r="113" spans="7:10">
-      <c r="G113" s="5"/>
+      <c r="J112" s="5"/>
+      <c r="K112" s="2"/>
+    </row>
+    <row r="113" spans="8:11">
       <c r="H113" s="5"/>
       <c r="I113" s="5"/>
-      <c r="J113" s="2"/>
-    </row>
-    <row r="114" spans="7:10">
-      <c r="G114" s="5"/>
+      <c r="J113" s="5"/>
+      <c r="K113" s="2"/>
+    </row>
+    <row r="114" spans="8:11">
       <c r="H114" s="5"/>
       <c r="I114" s="5"/>
-      <c r="J114" s="2"/>
-    </row>
-    <row r="115" spans="7:10">
-      <c r="G115" s="5"/>
+      <c r="J114" s="5"/>
+      <c r="K114" s="2"/>
+    </row>
+    <row r="115" spans="8:11">
       <c r="H115" s="5"/>
       <c r="I115" s="5"/>
-      <c r="J115" s="2"/>
-    </row>
-    <row r="116" spans="7:10">
-      <c r="G116" s="5"/>
+      <c r="J115" s="5"/>
+      <c r="K115" s="2"/>
+    </row>
+    <row r="116" spans="8:11">
       <c r="H116" s="5"/>
       <c r="I116" s="5"/>
-      <c r="J116" s="2"/>
-    </row>
-    <row r="117" spans="7:10">
-      <c r="G117" s="5"/>
+      <c r="J116" s="5"/>
+      <c r="K116" s="2"/>
+    </row>
+    <row r="117" spans="8:11">
       <c r="H117" s="5"/>
       <c r="I117" s="5"/>
-      <c r="J117" s="2"/>
-    </row>
-    <row r="118" spans="7:10">
-      <c r="G118" s="5"/>
+      <c r="J117" s="5"/>
+      <c r="K117" s="2"/>
+    </row>
+    <row r="118" spans="8:11">
       <c r="H118" s="5"/>
       <c r="I118" s="5"/>
-      <c r="J118" s="2"/>
-    </row>
-    <row r="119" spans="7:10">
-      <c r="G119" s="5"/>
+      <c r="J118" s="5"/>
+      <c r="K118" s="2"/>
+    </row>
+    <row r="119" spans="8:11">
       <c r="H119" s="5"/>
       <c r="I119" s="5"/>
-      <c r="J119" s="2"/>
-    </row>
-    <row r="120" spans="7:10">
-      <c r="G120" s="5"/>
+      <c r="J119" s="5"/>
+      <c r="K119" s="2"/>
+    </row>
+    <row r="120" spans="8:11">
       <c r="H120" s="5"/>
       <c r="I120" s="5"/>
-      <c r="J120" s="2"/>
-    </row>
-    <row r="121" spans="7:10">
-      <c r="G121" s="5"/>
+      <c r="J120" s="5"/>
+      <c r="K120" s="2"/>
+    </row>
+    <row r="121" spans="8:11">
       <c r="H121" s="5"/>
       <c r="I121" s="5"/>
-      <c r="J121" s="2"/>
-    </row>
-    <row r="122" spans="7:10">
-      <c r="G122" s="5"/>
+      <c r="J121" s="5"/>
+      <c r="K121" s="2"/>
+    </row>
+    <row r="122" spans="8:11">
       <c r="H122" s="5"/>
       <c r="I122" s="5"/>
-      <c r="J122" s="2"/>
-    </row>
-    <row r="123" spans="7:10">
-      <c r="G123" s="5"/>
+      <c r="J122" s="5"/>
+      <c r="K122" s="2"/>
+    </row>
+    <row r="123" spans="8:11">
       <c r="H123" s="5"/>
       <c r="I123" s="5"/>
-      <c r="J123" s="2"/>
-    </row>
-    <row r="124" spans="7:10">
-      <c r="G124" s="5"/>
+      <c r="J123" s="5"/>
+      <c r="K123" s="2"/>
+    </row>
+    <row r="124" spans="8:11">
       <c r="H124" s="5"/>
       <c r="I124" s="5"/>
-      <c r="J124" s="2"/>
-    </row>
-    <row r="125" spans="7:10">
-      <c r="G125" s="5"/>
+      <c r="J124" s="5"/>
+      <c r="K124" s="2"/>
+    </row>
+    <row r="125" spans="8:11">
       <c r="H125" s="5"/>
       <c r="I125" s="5"/>
-      <c r="J125" s="2"/>
-    </row>
-    <row r="126" spans="7:10">
-      <c r="G126" s="5"/>
+      <c r="J125" s="5"/>
+      <c r="K125" s="2"/>
+    </row>
+    <row r="126" spans="8:11">
       <c r="H126" s="5"/>
       <c r="I126" s="5"/>
-      <c r="J126" s="2"/>
-    </row>
-    <row r="127" spans="7:10">
-      <c r="G127" s="5"/>
+      <c r="J126" s="5"/>
+      <c r="K126" s="2"/>
+    </row>
+    <row r="127" spans="8:11">
       <c r="H127" s="5"/>
       <c r="I127" s="5"/>
-      <c r="J127" s="2"/>
-    </row>
-    <row r="128" spans="7:10">
-      <c r="G128" s="5"/>
+      <c r="J127" s="5"/>
+      <c r="K127" s="2"/>
+    </row>
+    <row r="128" spans="8:11">
       <c r="H128" s="5"/>
       <c r="I128" s="5"/>
-      <c r="J128" s="2"/>
-    </row>
-    <row r="129" spans="7:10">
-      <c r="G129" s="5"/>
+      <c r="J128" s="5"/>
+      <c r="K128" s="2"/>
+    </row>
+    <row r="129" spans="8:11">
       <c r="H129" s="5"/>
       <c r="I129" s="5"/>
-      <c r="J129" s="2"/>
+      <c r="J129" s="5"/>
+      <c r="K129" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5011,79 +5144,79 @@
           <x14:formula1>
             <xm:f>typeContribution!$A$1:$A$9</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E129</xm:sqref>
+          <xm:sqref>F2:F129</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Unknown value" error="Allowed values are listed in the corresponding sheet._x000a_" xr:uid="{A2274C7F-382B-DA4E-BA2D-99F2D43A77D1}">
           <x14:formula1>
             <xm:f>tadirahObject!$A$1:$A$36</xm:f>
           </x14:formula1>
-          <xm:sqref>N129</xm:sqref>
+          <xm:sqref>O129</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Unknown value" error="Allowed values are listed in the corresponding sheet._x000a_" xr:uid="{6209F047-5DDA-A245-916C-6E9B82CC088F}">
           <x14:formula1>
             <xm:f>tadirahActivity!$A$1:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>O129</xm:sqref>
+          <xm:sqref>P129</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Unknown value" error="Allowed values are listed in the corresponding sheet._x000a_" xr:uid="{D930787C-12C6-1F4C-A0DD-C09CB6587D61}">
           <x14:formula1>
             <xm:f>tadirahTechnique!$A$1:$A$34</xm:f>
           </x14:formula1>
-          <xm:sqref>P129</xm:sqref>
+          <xm:sqref>Q129</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Unknown value" error="A new value is allowed, but known values are preferred." xr:uid="{421566CA-4FCD-964E-924E-EBB90A31973F}">
           <x14:formula1>
             <xm:f>discipline!$A$1:$A$50</xm:f>
           </x14:formula1>
-          <xm:sqref>Q129</xm:sqref>
+          <xm:sqref>R129</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Unknown value" error="A new value is allowed, but known values are preferred." xr:uid="{9770751C-2A5D-8046-BE1F-E3C2E48A6EA3}">
           <x14:formula1>
             <xm:f>keyword!$A$1:$A$356</xm:f>
           </x14:formula1>
-          <xm:sqref>R129</xm:sqref>
+          <xm:sqref>S129</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Unknown value" error="Allowed values are listed in the corresponding sheet._x000a_" xr:uid="{7CFDB1DC-93F3-DA42-AC84-1BEEAFDBABE9}">
           <x14:formula1>
             <xm:f>vcc!$A$1:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>F129</xm:sqref>
+          <xm:sqref>G129</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="information" allowBlank="1" errorTitle="Unknown value" error="Allowed values are listed in the corresponding sheet._x000a_" xr:uid="{40FA88A0-7A49-9344-8535-91E358F450A4}">
           <x14:formula1>
             <xm:f>tadirahObject!$A$1:$A$36</xm:f>
           </x14:formula1>
-          <xm:sqref>N2:N128</xm:sqref>
+          <xm:sqref>O2:O128</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" errorTitle="Unknown value" error="Allowed values are listed in the corresponding sheet._x000a_" xr:uid="{8C924306-AB8B-B44B-A98B-608EAECD09B9}">
           <x14:formula1>
             <xm:f>vcc!$A$1:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F128</xm:sqref>
+          <xm:sqref>G2:G128</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" errorTitle="Unknown value" error="Allowed values are listed in the corresponding sheet._x000a_" xr:uid="{222BFBE5-934C-DB45-B6AB-9B57E6615960}">
           <x14:formula1>
             <xm:f>tadirahActivity!$A$1:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>O2:O128</xm:sqref>
+          <xm:sqref>P2:P128</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" errorTitle="Unknown value" error="Allowed values are listed in the corresponding sheet._x000a_" xr:uid="{D5B27ABF-9442-DF44-ADCD-B496A7B928D8}">
           <x14:formula1>
             <xm:f>tadirahTechnique!$A$1:$A$34</xm:f>
           </x14:formula1>
-          <xm:sqref>P2:P128</xm:sqref>
+          <xm:sqref>Q2:Q128</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" errorTitle="Unknown value" error="A new value is allowed, but known values are preferred." xr:uid="{F860FAFC-500B-9C4A-B8A8-DCD2368E2CED}">
           <x14:formula1>
             <xm:f>discipline!$A$1:$A$50</xm:f>
           </x14:formula1>
-          <xm:sqref>Q2:Q128</xm:sqref>
+          <xm:sqref>R2:R128</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" errorTitle="Unknown value" error="A new value is allowed, but known values are preferred." xr:uid="{DAD5E44B-0C24-4545-A982-00C9CCBD0ADE}">
           <x14:formula1>
             <xm:f>keyword!$A$1:$A$356</xm:f>
           </x14:formula1>
-          <xm:sqref>R2:R128</xm:sqref>
+          <xm:sqref>S2:S128</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
bulkimport: cost renamed to costTotal
</commit_message>
<xml_diff>
--- a/import/bulkTemplate.xlsx
+++ b/import/bulkTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10615"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dirk/github/Dans-labs/dariah-contrib/import/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A69EF5-0E19-8447-9EC2-DC0BFA005405}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA02FAB2-25DA-D540-A4D9-B7230BC4EC7B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="14620" windowWidth="51200" windowHeight="14180" xr2:uid="{9E4E58A0-E663-B14C-8CE3-230EC566B6AD}"/>
+    <workbookView xWindow="0" yWindow="14620" windowWidth="51200" windowHeight="14180" activeTab="2" xr2:uid="{9E4E58A0-E663-B14C-8CE3-230EC566B6AD}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="9" r:id="rId1"/>
@@ -1531,9 +1531,6 @@
   </si>
   <si>
     <t>About</t>
-  </si>
-  <si>
-    <t>cost</t>
   </si>
   <si>
     <t>costDescription</t>
@@ -1873,6 +1870,9 @@
 Your EPPN is visible on the interface when you are logged in: click the triangle in front of your name in the top right corner.
 </t>
     </r>
+  </si>
+  <si>
+    <t>costTotal</t>
   </si>
 </sst>
 </file>
@@ -2270,7 +2270,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06979413-2D2E-A04C-B6B8-B332E67D4E2B}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -2288,7 +2288,7 @@
         <v>498</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -2298,15 +2298,15 @@
         <v>495</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17">
       <c r="C3" s="7" t="s">
+        <v>504</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>505</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17">
@@ -4135,15 +4135,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>506</v>
+      </c>
+      <c r="B1" t="s">
         <v>507</v>
-      </c>
-      <c r="B1" t="s">
-        <v>508</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B2" t="s">
         <v>181</v>
@@ -4151,130 +4151,130 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
+        <v>509</v>
+      </c>
+      <c r="B3" t="s">
         <v>510</v>
-      </c>
-      <c r="B3" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
+        <v>511</v>
+      </c>
+      <c r="B4" t="s">
         <v>512</v>
-      </c>
-      <c r="B4" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
+        <v>539</v>
+      </c>
+      <c r="B5" t="s">
         <v>540</v>
-      </c>
-      <c r="B5" t="s">
-        <v>541</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
+        <v>513</v>
+      </c>
+      <c r="B6" t="s">
         <v>514</v>
-      </c>
-      <c r="B6" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
+        <v>515</v>
+      </c>
+      <c r="B7" t="s">
         <v>516</v>
-      </c>
-      <c r="B7" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
+        <v>517</v>
+      </c>
+      <c r="B8" t="s">
         <v>518</v>
-      </c>
-      <c r="B8" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
+        <v>519</v>
+      </c>
+      <c r="B9" t="s">
         <v>520</v>
-      </c>
-      <c r="B9" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
+        <v>521</v>
+      </c>
+      <c r="B10" t="s">
         <v>522</v>
-      </c>
-      <c r="B10" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
+        <v>523</v>
+      </c>
+      <c r="B11" t="s">
         <v>524</v>
-      </c>
-      <c r="B11" t="s">
-        <v>525</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
+        <v>525</v>
+      </c>
+      <c r="B12" t="s">
         <v>526</v>
-      </c>
-      <c r="B12" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
+        <v>527</v>
+      </c>
+      <c r="B13" t="s">
         <v>528</v>
-      </c>
-      <c r="B13" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
+        <v>529</v>
+      </c>
+      <c r="B14" t="s">
         <v>530</v>
-      </c>
-      <c r="B14" t="s">
-        <v>531</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
+        <v>531</v>
+      </c>
+      <c r="B15" t="s">
         <v>532</v>
-      </c>
-      <c r="B15" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
+        <v>533</v>
+      </c>
+      <c r="B16" t="s">
         <v>534</v>
-      </c>
-      <c r="B16" t="s">
-        <v>535</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
+        <v>535</v>
+      </c>
+      <c r="B17" t="s">
         <v>536</v>
-      </c>
-      <c r="B17" t="s">
-        <v>537</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
+        <v>537</v>
+      </c>
+      <c r="B18" t="s">
         <v>538</v>
-      </c>
-      <c r="B18" t="s">
-        <v>539</v>
       </c>
     </row>
   </sheetData>
@@ -4286,11 +4286,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{795743C0-90E8-1647-AA07-019994BABA6A}">
   <dimension ref="A1:S129"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="5" ySplit="1" topLeftCell="F92" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D94" sqref="D94"/>
+      <selection pane="bottomRight" activeCell="H95" sqref="H95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4310,16 +4310,16 @@
   <sheetData>
     <row r="1" spans="1:19" s="3" customFormat="1" ht="35" customHeight="1">
       <c r="A1" s="3" t="s">
+        <v>500</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>501</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>502</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>503</v>
-      </c>
       <c r="D1" s="3" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>0</v>
@@ -4334,10 +4334,10 @@
         <v>1</v>
       </c>
       <c r="I1" s="3" t="s">
+        <v>543</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>499</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>500</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
better checks for numerial bulk import
</commit_message>
<xml_diff>
--- a/import/bulkTemplate.xlsx
+++ b/import/bulkTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dirk/github/Dans-labs/dariah-contrib/import/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA02FAB2-25DA-D540-A4D9-B7230BC4EC7B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{965EDDD4-BF42-2E4E-B08B-AA751509994D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="14620" windowWidth="51200" windowHeight="14180" activeTab="2" xr2:uid="{9E4E58A0-E663-B14C-8CE3-230EC566B6AD}"/>
+    <workbookView xWindow="1320" yWindow="14620" windowWidth="49880" windowHeight="14180" activeTab="2" xr2:uid="{9E4E58A0-E663-B14C-8CE3-230EC566B6AD}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="9" r:id="rId1"/>
@@ -1660,6 +1660,9 @@
   </si>
   <si>
     <t>editors</t>
+  </si>
+  <si>
+    <t>costTotal</t>
   </si>
   <si>
     <r>
@@ -1855,7 +1858,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>cost</t>
+      <t>costTotal</t>
     </r>
     <r>
       <rPr>
@@ -1870,9 +1873,6 @@
 Your EPPN is visible on the interface when you are logged in: click the triangle in front of your name in the top right corner.
 </t>
     </r>
-  </si>
-  <si>
-    <t>costTotal</t>
   </si>
 </sst>
 </file>
@@ -2271,7 +2271,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2288,7 +2288,7 @@
         <v>498</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -4334,7 +4334,7 @@
         <v>1</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>499</v>

</xml_diff>